<commit_message>
Update auto laporan harian
Done:
1. Buat Laporan Auto report TS P2T Jam 18.00
2. Mengirim ke grup WA Tindak Lanjut JN max UID

To do :
1. Buat auto update laporan perubahan daya
2. Auto kirim laporan TS P2TL screenshoot Tabel Realisasi di python
</commit_message>
<xml_diff>
--- a/data/listuser/listuser.xlsx
+++ b/data/listuser/listuser.xlsx
@@ -1813,7 +1813,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
       <selection activeCell="L64" sqref="L64"/>
@@ -4381,6 +4381,32 @@
       <c r="F83" t="inlineStr">
         <is>
           <t>owner</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C84" t="n">
+        <v>32111</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Grup Laporan Dalsut</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>081321863455</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>admin</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Mengirim lap ts p2tl ke wa
berhasil mengirim lapopran TS P2TL ke WA

To do list :
Membuat laporan PD otomatis pada jam tertentu
</commit_message>
<xml_diff>
--- a/data/listuser/listuser.xlsx
+++ b/data/listuser/listuser.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CORE i7\Documents\GitHub\NEWASMENTE\data\listuser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DD17CC-5193-423A-8A25-0BB6B1F091E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F09596-61C4-4433-8565-5520F50181F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="323">
   <si>
     <t>NIP</t>
   </si>
@@ -928,6 +928,12 @@
   </si>
   <si>
     <t>081321863455</t>
+  </si>
+  <si>
+    <t>Pak Irhas</t>
+  </si>
+  <si>
+    <t>081278493630</t>
   </si>
   <si>
     <t>nama</t>
@@ -2279,10 +2285,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="M87" sqref="M87"/>
+      <selection activeCell="L91" sqref="L91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4277,6 +4283,32 @@
         <v>132</v>
       </c>
       <c r="H84">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>6167290309</v>
+      </c>
+      <c r="C85">
+        <v>32111</v>
+      </c>
+      <c r="D85" t="s">
+        <v>301</v>
+      </c>
+      <c r="E85" t="s">
+        <v>302</v>
+      </c>
+      <c r="F85" t="s">
+        <v>135</v>
+      </c>
+      <c r="G85" t="s">
+        <v>132</v>
+      </c>
+      <c r="H85">
         <v>32</v>
       </c>
     </row>
@@ -4306,7 +4338,7 @@
         <v>121</v>
       </c>
       <c r="C1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -4314,18 +4346,18 @@
         <v>1608202628</v>
       </c>
       <c r="C2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B3">
         <v>32640</v>
       </c>
       <c r="C3" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
@@ -4339,19 +4371,19 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B4">
         <v>32810</v>
       </c>
       <c r="C4" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
@@ -4363,10 +4395,10 @@
         <v>32810</v>
       </c>
       <c r="K4" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="L4" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="M4" t="s">
         <v>129</v>
@@ -4374,13 +4406,13 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B5">
         <v>32810</v>
       </c>
       <c r="C5" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
@@ -4398,10 +4430,10 @@
         <v>32810</v>
       </c>
       <c r="K5" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="M5" t="s">
         <v>129</v>
@@ -4415,10 +4447,10 @@
         <v>32810</v>
       </c>
       <c r="K6" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="L6" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="M6" t="s">
         <v>129</v>
@@ -4432,10 +4464,10 @@
         <v>32620</v>
       </c>
       <c r="K7" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="L7" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="M7" t="s">
         <v>179</v>
@@ -4783,16 +4815,16 @@
         <v>120</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>124</v>

</xml_diff>